<commit_message>
Day 4 – outcome: Implemented login, lab test selection, and cart flow scenarios
</commit_message>
<xml_diff>
--- a/target/test-classes/Exceldata/InputData.xlsx
+++ b/target/test-classes/Exceldata/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="9480"/>
+    <workbookView windowWidth="21000" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Samyuktha</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -42,14 +60,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,153 +516,154 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,33 +983,54 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.7777777777778"/>
+    <col min="1" max="1" width="12.8888888888889"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>7397783778</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>76457263</v>
+        <v>76755645454</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="abc@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>